<commit_message>
Finished the loading functions and documented them fully.
</commit_message>
<xml_diff>
--- a/SAMPLES/zz_lista_volontera_24_25.xlsx
+++ b/SAMPLES/zz_lista_volontera_24_25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lobel\Documents\Lobel\Zlatni Zmaj\Izvjesce\ZZ_Report_Analysis\SAMPLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD19528-16E6-4166-862F-B99419AF0EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A579CD3A-9333-4035-95E6-0378796246B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E4510751-5150-4AC6-8207-09F7448F3FDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{E4510751-5150-4AC6-8207-09F7448F3FDD}"/>
   </bookViews>
   <sheets>
     <sheet name="raspored" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="264">
   <si>
     <t>LOKACIJE</t>
   </si>
@@ -922,6 +922,9 @@
   </si>
   <si>
     <t>Laura Matić Zbiljski</t>
+  </si>
+  <si>
+    <t>ŠPANSKO (samo srijedom)</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1587,7 @@
   <dimension ref="B6:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1657,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>3</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1752,11 +1755,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71401D37-8643-4D80-AD6F-CCF38A0A6DA2}">
   <dimension ref="A1:AJ117"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="6" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,6 +1781,10 @@
         <f>COUNT(F:F)</f>
         <v>80</v>
       </c>
+      <c r="C1">
+        <f>B2/B6</f>
+        <v>4.8499999999999996</v>
+      </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1894,6 +1901,14 @@
       <c r="AJ7" s="9"/>
     </row>
     <row r="8" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>COUNTIF(E:E, "*~**")-A9</f>
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <f>B1-A8-2*A9</f>
+        <v>25</v>
+      </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
@@ -1959,6 +1974,10 @@
       </c>
     </row>
     <row r="9" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>COUNTIF(E:E, "*~*~**")</f>
+        <v>12</v>
+      </c>
       <c r="F9" t="s">
         <v>53</v>
       </c>
@@ -3152,10 +3171,10 @@
   <dimension ref="A1:AJ150"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="9" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,6 +3196,10 @@
         <f>COUNT(F:F)</f>
         <v>107</v>
       </c>
+      <c r="C1">
+        <f>B2/B6</f>
+        <v>8.9499999999999993</v>
+      </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3293,6 +3316,14 @@
       <c r="AJ7" s="9"/>
     </row>
     <row r="8" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>COUNTIF(E:E, "*~**")-A9</f>
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>B1-A8-2*A9</f>
+        <v>70</v>
+      </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
@@ -3358,6 +3389,10 @@
       </c>
     </row>
     <row r="9" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>COUNTIF(E:E, "*~*~**")</f>
+        <v>11</v>
+      </c>
       <c r="F9" t="s">
         <v>53</v>
       </c>
@@ -5067,11 +5102,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893FA989-93CF-494A-8578-57CB6CF43C39}">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="6" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5092,6 +5127,10 @@
       <c r="B1">
         <f>COUNT(F:F)</f>
         <v>54</v>
+      </c>
+      <c r="C1">
+        <f>B1/B6</f>
+        <v>7.7142857142857144</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -5183,6 +5222,14 @@
       <c r="AJ7" s="9"/>
     </row>
     <row r="8" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>COUNTIF(E:E, "*~**")-A9</f>
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <f>B1-A8-2*A9</f>
+        <v>16</v>
+      </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
@@ -5209,6 +5256,10 @@
       </c>
     </row>
     <row r="9" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>COUNTIF(E:E, "*~*~**")</f>
+        <v>11</v>
+      </c>
       <c r="F9" t="s">
         <v>53</v>
       </c>

</xml_diff>